<commit_message>
Loaded fresh datasets for week of 220530
</commit_message>
<xml_diff>
--- a/data/_input/static/metadata_summary_country.xlsx
+++ b/data/_input/static/metadata_summary_country.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dalberg\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dalberg\Documents\GitHub\covid19_vaccination_data\data\_input\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8026B7A6-7C8E-4E36-A782-5A7A416B0228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E568B0-3C0D-41EC-9DF5-42B5FEDCF4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{B7668904-28FE-4CEA-A556-9FF33A6F2EDC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B7668904-28FE-4CEA-A556-9FF33A6F2EDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="254">
-  <si>
-    <t>Category</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="271">
   <si>
     <t>Entity characteristics</t>
   </si>
@@ -250,9 +247,6 @@
     <t>Potential risk for expiry status</t>
   </si>
   <si>
-    <t>Categorical</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -271,15 +265,9 @@
     <t>Doses estimated remaining</t>
   </si>
   <si>
-    <t>Dose</t>
-  </si>
-  <si>
     <t>pu_del_rem_per</t>
   </si>
   <si>
-    <t>Doses estimated remaining, as percetnage of total population</t>
-  </si>
-  <si>
     <t>pu_del_rem_timeto</t>
   </si>
   <si>
@@ -322,9 +310,6 @@
     <t>adm_date_60p</t>
   </si>
   <si>
-    <t>Date of latest administration data reporting on individuals aged 60 and over</t>
-  </si>
-  <si>
     <t>eJRF and regional data systems</t>
   </si>
   <si>
@@ -352,24 +337,9 @@
     <t>adm_fv_adjust</t>
   </si>
   <si>
-    <t>Number of individuals with a complete primary series of any product of any source, with adustments for countries reporting adm_td and / or only adm_a1d and adm_td</t>
-  </si>
-  <si>
-    <t>Indivudals</t>
-  </si>
-  <si>
     <t>adm_fv_60p</t>
   </si>
   <si>
-    <t>Individuals aged 60 and older with a complete primary series</t>
-  </si>
-  <si>
-    <t>Individual</t>
-  </si>
-  <si>
-    <t>eJRF</t>
-  </si>
-  <si>
     <t>adm_fv_fem</t>
   </si>
   <si>
@@ -478,12 +448,6 @@
     <t>cov_60p_fv</t>
   </si>
   <si>
-    <t>Individuals aged 60 and older with a complete primary series, as percentage of population aged 60 and older</t>
-  </si>
-  <si>
-    <t>eJRF; UNPOP</t>
-  </si>
-  <si>
     <t>cov_hcw_fv</t>
   </si>
   <si>
@@ -574,9 +538,6 @@
     <t>ndvp_target</t>
   </si>
   <si>
-    <t>Coutry coverage target percentage</t>
-  </si>
-  <si>
     <t>ndvp_timeto</t>
   </si>
   <si>
@@ -673,18 +634,6 @@
     <t>Policy</t>
   </si>
   <si>
-    <t>pol_age_ado</t>
-  </si>
-  <si>
-    <t>Age group definiton, adolscents</t>
-  </si>
-  <si>
-    <t>eJRF; WHO Regional offices</t>
-  </si>
-  <si>
-    <t>Periodfically</t>
-  </si>
-  <si>
     <t>pol_age_old</t>
   </si>
   <si>
@@ -797,6 +746,108 @@
   </si>
   <si>
     <t>CoVDP</t>
+  </si>
+  <si>
+    <t>pop_older</t>
+  </si>
+  <si>
+    <t>Population, older adults (as defined by country)</t>
+  </si>
+  <si>
+    <t>UNPOP / eJRF</t>
+  </si>
+  <si>
+    <t>adm_a1d_hcw</t>
+  </si>
+  <si>
+    <t>adm_a1d_60p</t>
+  </si>
+  <si>
+    <t>adm_booster_hcw</t>
+  </si>
+  <si>
+    <t>adm_booster_60p</t>
+  </si>
+  <si>
+    <t>Number of booster and/or additional doses administered to healthcare workers</t>
+  </si>
+  <si>
+    <t>Number of booster and/or additional doses administered to older adults</t>
+  </si>
+  <si>
+    <t>Number of healthcare workers having received at least one dose</t>
+  </si>
+  <si>
+    <t>Number of older adults having received at least one dose</t>
+  </si>
+  <si>
+    <t>del_dose_jj_prop</t>
+  </si>
+  <si>
+    <t>Proportion of vaccine J&amp;J doses received of total vaccine doses received</t>
+  </si>
+  <si>
+    <t>cov_60p_a1d</t>
+  </si>
+  <si>
+    <t>cov_hcw_a1d</t>
+  </si>
+  <si>
+    <t>Older adults with a complete primary series, as percentage of older adult population</t>
+  </si>
+  <si>
+    <t>Older adults with at least one dose, as percentage of older adult population</t>
+  </si>
+  <si>
+    <t>Healthcare workers with at least one dose, as percentage of total healthcare worker population</t>
+  </si>
+  <si>
+    <t>adm_pv</t>
+  </si>
+  <si>
+    <t>Number of individuals with an incomplete (partial) primary series</t>
+  </si>
+  <si>
+    <t>Older adults with a complete primary series</t>
+  </si>
+  <si>
+    <t>pol_age_old_source</t>
+  </si>
+  <si>
+    <t>Character</t>
+  </si>
+  <si>
+    <t>adm_target_60p</t>
+  </si>
+  <si>
+    <t>adm_target_hcw</t>
+  </si>
+  <si>
+    <t>Number of healthcare workers targeted for COVID-19 vaccination, country-reported</t>
+  </si>
+  <si>
+    <t>Number of older adults targeted for COVID-19 vaccination, country-reported</t>
+  </si>
+  <si>
+    <t>Date of latest administration data reporting on older adults</t>
+  </si>
+  <si>
+    <t>Country coverage target percentage</t>
+  </si>
+  <si>
+    <t>Number of individuals with a complete primary series of any product of any source, with adjustments for countries reporting adm_td and / or only adm_a1d and adm_td</t>
+  </si>
+  <si>
+    <t>Source of older adults age group definition</t>
+  </si>
+  <si>
+    <t>Doses estimated remaining, as percentage of total population</t>
+  </si>
+  <si>
+    <t>eJRF and regional data systems; UNPOP</t>
+  </si>
+  <si>
+    <t>eJRF and regional data systems; WHO Regional offices</t>
   </si>
 </sst>
 </file>
@@ -856,16 +907,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -876,6 +959,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C9D72A3-FBB0-4A6C-9AD4-07FF5629FFA4}" name="Table1" displayName="Table1" ref="A1:H104" totalsRowShown="0">
+  <autoFilter ref="A1:H104" xr:uid="{8C9D72A3-FBB0-4A6C-9AD4-07FF5629FFA4}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{17BC83DA-7B1E-48E0-AFF2-9131F1A12296}" name="indicator"/>
+    <tableColumn id="2" xr3:uid="{2564B6D3-1653-4CD0-8192-CA07F90F47C6}" name="description" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{06B310F0-6888-4477-9B7B-C53BA0EF1B1E}" name="data_category" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{9DFA806B-7ADE-42FF-903F-5BC17F341DC1}" name="class"/>
+    <tableColumn id="5" xr3:uid="{AA85435F-FDF6-4ACB-84B1-35B025468717}" name="type"/>
+    <tableColumn id="6" xr3:uid="{CAA9EFB1-9A33-456E-87D7-E603F34F2680}" name="unit"/>
+    <tableColumn id="7" xr3:uid="{A5313499-9305-4184-8A1B-E3EDA1430DEB}" name="sources"/>
+    <tableColumn id="8" xr3:uid="{F50AF624-F8AD-452D-AAA1-FC5DA6E3A362}" name="update_frequency"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1175,2431 +1275,2731 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07602C46-AF60-4A59-9AEF-A3C5225522E1}">
-  <dimension ref="A1:H93"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="8" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.90625" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="80.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="B1" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="C1" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="D1" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="E1" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="F1" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="G1" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="H1" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>241</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>247</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="H3" t="s">
-        <v>8</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>240</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>246</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>243</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>245</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>242</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>244</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="H7" t="s">
-        <v>8</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="E8" t="s">
-        <v>5</v>
-      </c>
       <c r="F8" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H8" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>264</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G9" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="H9" t="s">
-        <v>8</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" t="s">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
         <v>4</v>
       </c>
-      <c r="E11" t="s">
-        <v>25</v>
-      </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G11" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>98</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
         <v>4</v>
       </c>
-      <c r="E12" t="s">
-        <v>25</v>
-      </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="H12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>257</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
         <v>4</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>5</v>
       </c>
-      <c r="F13" t="s">
-        <v>26</v>
-      </c>
       <c r="G13" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="H13" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>266</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="G14" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="H14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
         <v>4</v>
       </c>
-      <c r="E15" t="s">
-        <v>25</v>
-      </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="G15" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="H15" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
         <v>4</v>
       </c>
-      <c r="E16" t="s">
-        <v>25</v>
-      </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="G16" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="H16" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
         <v>4</v>
       </c>
-      <c r="E17" t="s">
-        <v>25</v>
-      </c>
       <c r="F17" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="G17" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="H17" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>255</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="G18" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="H18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>260</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>263</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
         <v>4</v>
       </c>
-      <c r="E19" t="s">
-        <v>25</v>
-      </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="G19" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="H19" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>261</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>262</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
         <v>5</v>
       </c>
-      <c r="F20" t="s">
-        <v>30</v>
-      </c>
       <c r="G20" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="H20" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="B21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
         <v>60</v>
       </c>
-      <c r="C21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" t="s">
-        <v>61</v>
-      </c>
       <c r="G21" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="H21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>223</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>224</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
+        <v>259</v>
+      </c>
+      <c r="E22" t="s">
         <v>4</v>
       </c>
-      <c r="E22" t="s">
-        <v>5</v>
-      </c>
       <c r="F22" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G22" t="s">
-        <v>52</v>
+        <v>236</v>
       </c>
       <c r="H22" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>250</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>253</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>135</v>
       </c>
       <c r="D23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F23" t="s">
-        <v>26</v>
+        <v>124</v>
       </c>
       <c r="G23" t="s">
-        <v>52</v>
+        <v>269</v>
       </c>
       <c r="H23" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>136</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>252</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>135</v>
       </c>
       <c r="D24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F24" t="s">
-        <v>26</v>
+        <v>124</v>
       </c>
       <c r="G24" t="s">
-        <v>52</v>
+        <v>269</v>
       </c>
       <c r="H24" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>251</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>254</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="D25" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F25" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="G25" t="s">
-        <v>73</v>
+        <v>269</v>
       </c>
       <c r="H25" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>138</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="D26" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F26" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="G26" t="s">
-        <v>73</v>
+        <v>139</v>
       </c>
       <c r="H26" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>140</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>141</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="D27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F27" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="G27" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="H27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="D28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G28" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="H28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>144</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>145</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="D29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F29" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
       <c r="G29" t="s">
-        <v>73</v>
+        <v>269</v>
       </c>
       <c r="H29" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>146</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="D30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G30" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="H30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>149</v>
       </c>
       <c r="C31" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="D31" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F31" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="G31" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="H31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>151</v>
       </c>
       <c r="C32" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="D32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F32" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="G32" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="H32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>152</v>
+      </c>
+      <c r="B33" t="s">
+        <v>153</v>
+      </c>
+      <c r="C33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" t="s">
+        <v>124</v>
+      </c>
+      <c r="G33" t="s">
+        <v>269</v>
+      </c>
+      <c r="H33" t="s">
         <v>92</v>
-      </c>
-      <c r="B33" t="s">
-        <v>93</v>
-      </c>
-      <c r="C33" t="s">
-        <v>86</v>
-      </c>
-      <c r="D33" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33" t="s">
-        <v>30</v>
-      </c>
-      <c r="G33" t="s">
-        <v>89</v>
-      </c>
-      <c r="H33" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>154</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>155</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="D34" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F34" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="G34" t="s">
-        <v>96</v>
+        <v>269</v>
       </c>
       <c r="H34" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>98</v>
-      </c>
-      <c r="B35" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" t="s">
-        <v>86</v>
+        <v>221</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>30</v>
+        <v>259</v>
       </c>
       <c r="E35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="G35" t="s">
-        <v>96</v>
+        <v>235</v>
       </c>
       <c r="H35" t="s">
-        <v>97</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>50</v>
       </c>
       <c r="C36" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="D36" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E36" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F36" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G36" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="H36" t="s">
-        <v>97</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="D37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F37" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="G37" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="H37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="D38" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F38" t="s">
-        <v>106</v>
+        <v>37</v>
       </c>
       <c r="G38" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="H38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>108</v>
+        <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="D39" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" t="s">
         <v>4</v>
       </c>
-      <c r="E39" t="s">
-        <v>5</v>
-      </c>
       <c r="F39" t="s">
-        <v>109</v>
+        <v>29</v>
       </c>
       <c r="G39" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="H39" t="s">
-        <v>97</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="B40" t="s">
-        <v>112</v>
+        <v>249</v>
       </c>
       <c r="C40" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="D40" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E40" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F40" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="G40" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="H40" t="s">
-        <v>97</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>114</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="D41" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F41" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
       <c r="G41" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="H41" t="s">
-        <v>97</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="D42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s">
         <v>4</v>
       </c>
-      <c r="E42" t="s">
-        <v>5</v>
-      </c>
       <c r="F42" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
       <c r="G42" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="H42" t="s">
-        <v>97</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B43" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C43" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="D43" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E43" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F43" t="s">
-        <v>61</v>
+        <v>116</v>
       </c>
       <c r="G43" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B44" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C44" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="D44" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F44" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="G44" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>119</v>
+      </c>
+      <c r="B45" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45" t="s">
+        <v>113</v>
+      </c>
+      <c r="D45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" t="s">
         <v>121</v>
       </c>
-      <c r="B45" t="s">
-        <v>122</v>
-      </c>
-      <c r="C45" t="s">
-        <v>86</v>
-      </c>
-      <c r="D45" t="s">
-        <v>4</v>
-      </c>
-      <c r="E45" t="s">
-        <v>25</v>
-      </c>
-      <c r="F45" t="s">
-        <v>26</v>
-      </c>
       <c r="G45" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>122</v>
+      </c>
+      <c r="B46" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" t="s">
         <v>124</v>
       </c>
-      <c r="B46" t="s">
-        <v>125</v>
-      </c>
-      <c r="C46" t="s">
-        <v>123</v>
-      </c>
-      <c r="D46" t="s">
-        <v>4</v>
-      </c>
-      <c r="E46" t="s">
-        <v>25</v>
-      </c>
-      <c r="F46" t="s">
-        <v>126</v>
-      </c>
       <c r="G46" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B47" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C47" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D47" t="s">
-        <v>4</v>
+        <v>259</v>
       </c>
       <c r="E47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F47" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="G47" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B48" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C48" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D48" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F48" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="G48" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>129</v>
+      </c>
+      <c r="B49" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49" t="s">
+        <v>113</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" t="s">
+        <v>131</v>
+      </c>
+      <c r="G49" t="s">
         <v>132</v>
       </c>
-      <c r="B49" t="s">
-        <v>133</v>
-      </c>
-      <c r="C49" t="s">
-        <v>123</v>
-      </c>
-      <c r="D49" t="s">
-        <v>4</v>
-      </c>
-      <c r="E49" t="s">
-        <v>25</v>
-      </c>
-      <c r="F49" t="s">
-        <v>134</v>
-      </c>
-      <c r="G49" t="s">
-        <v>89</v>
-      </c>
       <c r="H49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B50" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C50" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D50" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="E50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F50" t="s">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="G50" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="H50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>137</v>
+        <v>68</v>
       </c>
       <c r="B51" t="s">
-        <v>138</v>
+        <v>69</v>
       </c>
       <c r="C51" t="s">
-        <v>123</v>
+        <v>67</v>
       </c>
       <c r="D51" t="s">
-        <v>4</v>
+        <v>259</v>
       </c>
       <c r="E51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F51" t="s">
-        <v>131</v>
+        <v>70</v>
       </c>
       <c r="G51" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="H51" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>139</v>
+        <v>72</v>
       </c>
       <c r="B52" t="s">
-        <v>140</v>
+        <v>73</v>
       </c>
       <c r="C52" t="s">
-        <v>123</v>
+        <v>67</v>
       </c>
       <c r="D52" t="s">
-        <v>4</v>
+        <v>259</v>
       </c>
       <c r="E52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F52" t="s">
-        <v>141</v>
+        <v>70</v>
       </c>
       <c r="G52" t="s">
-        <v>142</v>
+        <v>71</v>
       </c>
       <c r="H52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>143</v>
+        <v>190</v>
       </c>
       <c r="B53" t="s">
-        <v>144</v>
+        <v>191</v>
       </c>
       <c r="C53" t="s">
-        <v>123</v>
+        <v>189</v>
       </c>
       <c r="D53" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F53" t="s">
-        <v>141</v>
+        <v>192</v>
       </c>
       <c r="G53" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="H53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="B54" t="s">
-        <v>147</v>
+        <v>195</v>
       </c>
       <c r="C54" t="s">
-        <v>145</v>
+        <v>189</v>
       </c>
       <c r="D54" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" t="s">
         <v>4</v>
       </c>
-      <c r="E54" t="s">
-        <v>25</v>
-      </c>
       <c r="F54" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
       <c r="G54" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="H54" t="s">
-        <v>97</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>149</v>
-      </c>
-      <c r="B55" t="s">
-        <v>150</v>
-      </c>
-      <c r="C55" t="s">
-        <v>145</v>
+        <v>220</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="D55" t="s">
+        <v>259</v>
+      </c>
+      <c r="E55" t="s">
         <v>4</v>
       </c>
-      <c r="E55" t="s">
-        <v>25</v>
-      </c>
       <c r="F55" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="G55" t="s">
-        <v>151</v>
+        <v>234</v>
       </c>
       <c r="H55" t="s">
-        <v>97</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>152</v>
+        <v>222</v>
       </c>
       <c r="B56" t="s">
-        <v>153</v>
+        <v>225</v>
       </c>
       <c r="C56" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="D56" t="s">
+        <v>230</v>
+      </c>
+      <c r="E56" t="s">
         <v>4</v>
       </c>
-      <c r="E56" t="s">
-        <v>25</v>
-      </c>
       <c r="F56" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="G56" t="s">
-        <v>142</v>
+        <v>233</v>
       </c>
       <c r="H56" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B57" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C57" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D57" t="s">
+        <v>29</v>
+      </c>
+      <c r="E57" t="s">
         <v>4</v>
       </c>
-      <c r="E57" t="s">
-        <v>25</v>
-      </c>
       <c r="F57" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G57" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="H57" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B58" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C58" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D58" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F58" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="G58" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="H58" t="s">
-        <v>97</v>
+        <v>31</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B59" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C59" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D59" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E59" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F59" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="G59" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="H59" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B60" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C60" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D60" t="s">
-        <v>4</v>
+        <v>259</v>
       </c>
       <c r="E60" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F60" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="G60" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="H60" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B61" t="s">
-        <v>163</v>
+        <v>265</v>
       </c>
       <c r="C61" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D61" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" t="s">
         <v>4</v>
       </c>
-      <c r="E61" t="s">
-        <v>25</v>
-      </c>
       <c r="F61" t="s">
-        <v>38</v>
+        <v>124</v>
       </c>
       <c r="G61" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="H61" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B62" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C62" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D62" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E62" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F62" t="s">
-        <v>134</v>
+        <v>79</v>
       </c>
       <c r="G62" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="H62" t="s">
-        <v>97</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>166</v>
-      </c>
-      <c r="B63" t="s">
-        <v>167</v>
-      </c>
-      <c r="C63" t="s">
-        <v>145</v>
+        <v>199</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="D63" t="s">
+        <v>259</v>
+      </c>
+      <c r="E63" t="s">
         <v>4</v>
       </c>
-      <c r="E63" t="s">
-        <v>25</v>
-      </c>
       <c r="F63" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="G63" t="s">
-        <v>148</v>
+        <v>270</v>
       </c>
       <c r="H63" t="s">
-        <v>97</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>168</v>
-      </c>
-      <c r="B64" t="s">
-        <v>169</v>
-      </c>
-      <c r="C64" t="s">
-        <v>145</v>
+        <v>258</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="D64" t="s">
-        <v>30</v>
+        <v>259</v>
       </c>
       <c r="E64" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="G64" t="s">
-        <v>170</v>
+        <v>270</v>
       </c>
       <c r="H64" t="s">
-        <v>171</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>172</v>
-      </c>
-      <c r="B65" t="s">
-        <v>173</v>
-      </c>
-      <c r="C65" t="s">
-        <v>145</v>
+        <v>201</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="D65" t="s">
+        <v>259</v>
+      </c>
+      <c r="E65" t="s">
         <v>4</v>
       </c>
-      <c r="E65" t="s">
-        <v>25</v>
-      </c>
       <c r="F65" t="s">
-        <v>131</v>
+        <v>70</v>
       </c>
       <c r="G65" t="s">
-        <v>142</v>
+        <v>270</v>
       </c>
       <c r="H65" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>174</v>
+        <v>1</v>
       </c>
       <c r="B66" t="s">
-        <v>175</v>
+        <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
+        <v>3</v>
+      </c>
+      <c r="E66" t="s">
         <v>4</v>
       </c>
-      <c r="E66" t="s">
-        <v>25</v>
-      </c>
       <c r="F66" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="G66" t="s">
-        <v>142</v>
+        <v>6</v>
       </c>
       <c r="H66" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>176</v>
+        <v>8</v>
       </c>
       <c r="B67" t="s">
-        <v>177</v>
+        <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="D67" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="E67" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="F67" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="G67" t="s">
-        <v>142</v>
+        <v>6</v>
       </c>
       <c r="H67" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>178</v>
+        <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>179</v>
+        <v>11</v>
       </c>
       <c r="C68" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" t="s">
         <v>4</v>
       </c>
-      <c r="E68" t="s">
+      <c r="F68" t="s">
         <v>5</v>
       </c>
-      <c r="F68" t="s">
-        <v>134</v>
-      </c>
       <c r="G68" t="s">
-        <v>170</v>
+        <v>6</v>
       </c>
       <c r="H68" t="s">
-        <v>171</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>180</v>
-      </c>
-      <c r="B69" t="s">
-        <v>181</v>
-      </c>
-      <c r="C69" t="s">
-        <v>145</v>
+        <v>207</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E69" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F69" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="G69" t="s">
-        <v>142</v>
+        <v>6</v>
       </c>
       <c r="H69" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>182</v>
+        <v>12</v>
       </c>
       <c r="B70" t="s">
-        <v>183</v>
+        <v>13</v>
       </c>
       <c r="C70" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="E70" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="F70" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="G70" t="s">
-        <v>142</v>
+        <v>6</v>
       </c>
       <c r="H70" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>184</v>
+        <v>14</v>
       </c>
       <c r="B71" t="s">
-        <v>185</v>
+        <v>15</v>
       </c>
       <c r="C71" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="D71" t="s">
+        <v>3</v>
+      </c>
+      <c r="E71" t="s">
         <v>4</v>
       </c>
-      <c r="E71" t="s">
-        <v>25</v>
-      </c>
       <c r="F71" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="G71" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
       <c r="H71" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>186</v>
+        <v>18</v>
       </c>
       <c r="B72" t="s">
-        <v>187</v>
+        <v>19</v>
       </c>
       <c r="C72" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="E72" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="F72" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="G72" t="s">
-        <v>142</v>
+        <v>6</v>
       </c>
       <c r="H72" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>188</v>
+        <v>237</v>
       </c>
       <c r="B73" t="s">
-        <v>189</v>
+        <v>238</v>
       </c>
       <c r="C73" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="D73" t="s">
+        <v>3</v>
+      </c>
+      <c r="E73" t="s">
         <v>4</v>
       </c>
-      <c r="E73" t="s">
-        <v>25</v>
-      </c>
       <c r="F73" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="G73" t="s">
-        <v>142</v>
+        <v>239</v>
       </c>
       <c r="H73" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>190</v>
+        <v>20</v>
       </c>
       <c r="B74" t="s">
-        <v>191</v>
+        <v>21</v>
       </c>
       <c r="C74" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="D74" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="E74" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="F74" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="G74" t="s">
-        <v>142</v>
+        <v>6</v>
       </c>
       <c r="H74" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>192</v>
+        <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>193</v>
+        <v>75</v>
       </c>
       <c r="C75" t="s">
-        <v>145</v>
+        <v>67</v>
       </c>
       <c r="D75" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E75" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F75" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="G75" t="s">
-        <v>142</v>
+        <v>71</v>
       </c>
       <c r="H75" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>194</v>
+        <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>195</v>
+        <v>268</v>
       </c>
       <c r="C76" t="s">
-        <v>145</v>
+        <v>67</v>
       </c>
       <c r="D76" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E76" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F76" t="s">
-        <v>131</v>
+        <v>37</v>
       </c>
       <c r="G76" t="s">
-        <v>142</v>
+        <v>71</v>
       </c>
       <c r="H76" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>196</v>
+        <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>197</v>
+        <v>78</v>
       </c>
       <c r="C77" t="s">
-        <v>145</v>
+        <v>67</v>
       </c>
       <c r="D77" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E77" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F77" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="G77" t="s">
-        <v>142</v>
+        <v>71</v>
       </c>
       <c r="H77" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>198</v>
+        <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>199</v>
+        <v>81</v>
       </c>
       <c r="C78" t="s">
-        <v>145</v>
+        <v>67</v>
       </c>
       <c r="D78" t="s">
+        <v>3</v>
+      </c>
+      <c r="E78" t="s">
+        <v>24</v>
+      </c>
+      <c r="F78" t="s">
+        <v>37</v>
+      </c>
+      <c r="G78" t="s">
         <v>71</v>
       </c>
-      <c r="E78" t="s">
-        <v>25</v>
-      </c>
-      <c r="F78" t="s">
-        <v>72</v>
-      </c>
-      <c r="G78" t="s">
-        <v>142</v>
-      </c>
       <c r="H78" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>200</v>
-      </c>
-      <c r="B79" t="s">
-        <v>201</v>
-      </c>
-      <c r="C79" t="s">
-        <v>145</v>
+        <v>204</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="D79" t="s">
+        <v>29</v>
+      </c>
+      <c r="E79" t="s">
         <v>4</v>
       </c>
-      <c r="E79" t="s">
-        <v>25</v>
-      </c>
       <c r="F79" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="G79" t="s">
-        <v>142</v>
+        <v>206</v>
       </c>
       <c r="H79" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>203</v>
+        <v>27</v>
       </c>
       <c r="B80" t="s">
-        <v>204</v>
+        <v>28</v>
       </c>
       <c r="C80" t="s">
-        <v>202</v>
+        <v>26</v>
       </c>
       <c r="D80" t="s">
+        <v>29</v>
+      </c>
+      <c r="E80" t="s">
         <v>4</v>
       </c>
-      <c r="E80" t="s">
-        <v>25</v>
-      </c>
       <c r="F80" t="s">
-        <v>205</v>
+        <v>29</v>
       </c>
       <c r="G80" t="s">
-        <v>206</v>
+        <v>30</v>
       </c>
       <c r="H80" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>207</v>
+        <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>208</v>
+        <v>33</v>
       </c>
       <c r="C81" t="s">
-        <v>202</v>
+        <v>26</v>
       </c>
       <c r="D81" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E81" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F81" t="s">
-        <v>209</v>
+        <v>25</v>
       </c>
       <c r="G81" t="s">
-        <v>210</v>
+        <v>34</v>
       </c>
       <c r="H81" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>212</v>
+        <v>35</v>
       </c>
       <c r="B82" t="s">
-        <v>213</v>
+        <v>36</v>
       </c>
       <c r="C82" t="s">
-        <v>211</v>
+        <v>26</v>
       </c>
       <c r="D82" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="E82" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F82" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="G82" t="s">
-        <v>214</v>
+        <v>38</v>
       </c>
       <c r="H82" t="s">
-        <v>215</v>
+        <v>31</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>216</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>211</v>
+        <v>39</v>
+      </c>
+      <c r="B83" t="s">
+        <v>40</v>
+      </c>
+      <c r="C83" t="s">
+        <v>26</v>
       </c>
       <c r="D83" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="E83" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="G83" t="s">
-        <v>214</v>
+        <v>30</v>
       </c>
       <c r="H83" t="s">
-        <v>215</v>
+        <v>31</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>218</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>211</v>
+        <v>41</v>
+      </c>
+      <c r="B84" t="s">
+        <v>42</v>
+      </c>
+      <c r="C84" t="s">
+        <v>26</v>
       </c>
       <c r="D84" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="E84" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F84" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="G84" t="s">
-        <v>214</v>
+        <v>43</v>
       </c>
       <c r="H84" t="s">
-        <v>215</v>
+        <v>31</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>221</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>220</v>
+        <v>169</v>
+      </c>
+      <c r="B85" t="s">
+        <v>170</v>
+      </c>
+      <c r="C85" t="s">
+        <v>135</v>
       </c>
       <c r="D85" t="s">
-        <v>30</v>
+        <v>259</v>
       </c>
       <c r="E85" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F85" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="G85" t="s">
-        <v>223</v>
+        <v>132</v>
       </c>
       <c r="H85" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>224</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C86" s="1"/>
+        <v>171</v>
+      </c>
+      <c r="B86" t="s">
+        <v>172</v>
+      </c>
+      <c r="C86" t="s">
+        <v>135</v>
+      </c>
       <c r="D86" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E86" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F86" t="s">
-        <v>6</v>
+        <v>79</v>
       </c>
       <c r="G86" t="s">
-        <v>7</v>
+        <v>132</v>
       </c>
       <c r="H86" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>226</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C87" s="1"/>
+        <v>173</v>
+      </c>
+      <c r="B87" t="s">
+        <v>174</v>
+      </c>
+      <c r="C87" t="s">
+        <v>135</v>
+      </c>
       <c r="D87" t="s">
-        <v>4</v>
+        <v>259</v>
       </c>
       <c r="E87" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F87" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="G87" t="s">
-        <v>7</v>
+        <v>132</v>
       </c>
       <c r="H87" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>235</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>1</v>
+        <v>175</v>
+      </c>
+      <c r="B88" t="s">
+        <v>176</v>
+      </c>
+      <c r="C88" t="s">
+        <v>135</v>
       </c>
       <c r="D88" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="E88" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F88" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="G88" t="s">
-        <v>248</v>
+        <v>132</v>
       </c>
       <c r="H88" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>236</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>1</v>
+        <v>109</v>
+      </c>
+      <c r="B89" t="s">
+        <v>110</v>
+      </c>
+      <c r="C89" t="s">
+        <v>82</v>
       </c>
       <c r="D89" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="E89" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F89" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="G89" t="s">
-        <v>249</v>
+        <v>85</v>
       </c>
       <c r="H89" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>237</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="B90" t="s">
+        <v>64</v>
+      </c>
+      <c r="C90" t="s">
+        <v>48</v>
       </c>
       <c r="D90" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="E90" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F90" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="G90" t="s">
-        <v>251</v>
+        <v>51</v>
       </c>
       <c r="H90" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>238</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>1</v>
+        <v>44</v>
+      </c>
+      <c r="B91" t="s">
+        <v>45</v>
+      </c>
+      <c r="C91" t="s">
+        <v>26</v>
       </c>
       <c r="D91" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="E91" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F91" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="G91" t="s">
-        <v>252</v>
+        <v>30</v>
       </c>
       <c r="H91" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>239</v>
+        <v>22</v>
       </c>
       <c r="B92" t="s">
-        <v>242</v>
+        <v>23</v>
       </c>
       <c r="C92" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
-        <v>247</v>
+        <v>3</v>
       </c>
       <c r="E92" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F92" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="G92" t="s">
-        <v>250</v>
+        <v>6</v>
       </c>
       <c r="H92" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>240</v>
+        <v>177</v>
       </c>
       <c r="B93" t="s">
-        <v>241</v>
+        <v>178</v>
       </c>
       <c r="C93" t="s">
-        <v>1</v>
+        <v>135</v>
       </c>
       <c r="D93" t="s">
-        <v>71</v>
+        <v>259</v>
       </c>
       <c r="E93" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F93" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G93" t="s">
-        <v>253</v>
+        <v>132</v>
       </c>
       <c r="H93" t="s">
-        <v>18</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>179</v>
+      </c>
+      <c r="B94" t="s">
+        <v>180</v>
+      </c>
+      <c r="C94" t="s">
+        <v>135</v>
+      </c>
+      <c r="D94" t="s">
+        <v>3</v>
+      </c>
+      <c r="E94" t="s">
+        <v>24</v>
+      </c>
+      <c r="F94" t="s">
+        <v>79</v>
+      </c>
+      <c r="G94" t="s">
+        <v>132</v>
+      </c>
+      <c r="H94" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>111</v>
+      </c>
+      <c r="B95" t="s">
+        <v>112</v>
+      </c>
+      <c r="C95" t="s">
+        <v>82</v>
+      </c>
+      <c r="D95" t="s">
+        <v>3</v>
+      </c>
+      <c r="E95" t="s">
+        <v>24</v>
+      </c>
+      <c r="F95" t="s">
+        <v>25</v>
+      </c>
+      <c r="G95" t="s">
+        <v>85</v>
+      </c>
+      <c r="H95" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>65</v>
+      </c>
+      <c r="B96" t="s">
+        <v>66</v>
+      </c>
+      <c r="C96" t="s">
+        <v>48</v>
+      </c>
+      <c r="D96" t="s">
+        <v>3</v>
+      </c>
+      <c r="E96" t="s">
+        <v>24</v>
+      </c>
+      <c r="F96" t="s">
+        <v>25</v>
+      </c>
+      <c r="G96" t="s">
+        <v>51</v>
+      </c>
+      <c r="H96" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>46</v>
+      </c>
+      <c r="B97" t="s">
+        <v>47</v>
+      </c>
+      <c r="C97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D97" t="s">
+        <v>3</v>
+      </c>
+      <c r="E97" t="s">
+        <v>24</v>
+      </c>
+      <c r="F97" t="s">
+        <v>25</v>
+      </c>
+      <c r="G97" t="s">
+        <v>30</v>
+      </c>
+      <c r="H97" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>209</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D98" t="s">
+        <v>3</v>
+      </c>
+      <c r="E98" t="s">
+        <v>24</v>
+      </c>
+      <c r="F98" t="s">
+        <v>25</v>
+      </c>
+      <c r="G98" t="s">
+        <v>6</v>
+      </c>
+      <c r="H98" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>181</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C99" t="s">
+        <v>135</v>
+      </c>
+      <c r="D99" t="s">
+        <v>3</v>
+      </c>
+      <c r="E99" t="s">
+        <v>24</v>
+      </c>
+      <c r="F99" t="s">
+        <v>121</v>
+      </c>
+      <c r="G99" t="s">
+        <v>132</v>
+      </c>
+      <c r="H99" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>183</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C100" t="s">
+        <v>135</v>
+      </c>
+      <c r="D100" t="s">
+        <v>3</v>
+      </c>
+      <c r="E100" t="s">
+        <v>24</v>
+      </c>
+      <c r="F100" t="s">
+        <v>70</v>
+      </c>
+      <c r="G100" t="s">
+        <v>132</v>
+      </c>
+      <c r="H100" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>185</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C101" t="s">
+        <v>135</v>
+      </c>
+      <c r="D101" t="s">
+        <v>259</v>
+      </c>
+      <c r="E101" t="s">
+        <v>24</v>
+      </c>
+      <c r="F101" t="s">
+        <v>70</v>
+      </c>
+      <c r="G101" t="s">
+        <v>132</v>
+      </c>
+      <c r="H101" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>187</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C102" t="s">
+        <v>135</v>
+      </c>
+      <c r="D102" t="s">
+        <v>3</v>
+      </c>
+      <c r="E102" t="s">
+        <v>24</v>
+      </c>
+      <c r="F102" t="s">
+        <v>79</v>
+      </c>
+      <c r="G102" t="s">
+        <v>132</v>
+      </c>
+      <c r="H102" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>219</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D103" t="s">
+        <v>259</v>
+      </c>
+      <c r="E103" t="s">
+        <v>4</v>
+      </c>
+      <c r="F103" t="s">
+        <v>70</v>
+      </c>
+      <c r="G103" t="s">
+        <v>232</v>
+      </c>
+      <c r="H103" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>218</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D104" t="s">
+        <v>259</v>
+      </c>
+      <c r="E104" t="s">
+        <v>4</v>
+      </c>
+      <c r="F104" t="s">
+        <v>70</v>
+      </c>
+      <c r="G104" t="s">
+        <v>231</v>
+      </c>
+      <c r="H104" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -3816,13 +4216,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D63D2C1-0846-45EC-92FC-C1A4009D583E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D63D2C1-0846-45EC-92FC-C1A4009D583E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b370a6fa-a798-42e0-969d-19c284d8683f"/>
+    <ds:schemaRef ds:uri="62ca1376-8bea-4949-825e-fec085c3924e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4627CB4-3356-4239-9CEE-5D697A543E8C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4627CB4-3356-4239-9CEE-5D697A543E8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9666D219-5436-480B-874A-B0985F4B1352}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9666D219-5436-480B-874A-B0985F4B1352}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>